<commit_message>
Keyboard enter button press, close current window, flipkart demo test case, addition dependancy shifted to conf.json file
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ni3\automation\PythonSelenium\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ni3\automation\PythonSelenium\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2F8734-0AEF-45C6-86AD-46D17D6E2993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B609AFC-2314-4DF1-B28E-80AE4EEA8D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="flipkart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>URL</t>
   </si>
@@ -29,6 +30,12 @@
   </si>
   <si>
     <t>https://www.amazon.in/</t>
+  </si>
+  <si>
+    <t>https://www.flipkart.com/</t>
+  </si>
+  <si>
+    <t>ASUS Vivobook</t>
   </si>
 </sst>
 </file>
@@ -398,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,8 +428,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>